<commit_message>
search new Phulchi school result
</commit_message>
<xml_diff>
--- a/src/test/java/com/qa/testdata/JAC_10th_Results.xlsx
+++ b/src/test/java/com/qa/testdata/JAC_10th_Results.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All My Core Programming\Testing-with-Java\JAC-RanchiResults\src\test\java\com\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F5D6A9-732E-489C-9D9B-FA202936B8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE72DD76-569D-4B59-ADC3-5475B3A057D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GCHSB" sheetId="1" r:id="rId1"/>
+    <sheet name="22097" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2400" uniqueCount="1372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2640" uniqueCount="1462">
   <si>
     <t>0001</t>
   </si>
@@ -4141,6 +4142,276 @@
   </si>
   <si>
     <t>Khemiya Devi</t>
+  </si>
+  <si>
+    <t>Chandan Kumar Ray</t>
+  </si>
+  <si>
+    <t>Birju Ray</t>
+  </si>
+  <si>
+    <t>Utkramit High School Phulchi Bharkatta</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.20                    </t>
+  </si>
+  <si>
+    <t>Ravi Ray</t>
+  </si>
+  <si>
+    <t>Dilip Ray</t>
+  </si>
+  <si>
+    <t>Jhunjhun Devi</t>
+  </si>
+  <si>
+    <t>339</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.80                    </t>
+  </si>
+  <si>
+    <t>Bhawani Kumari</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.60                    </t>
+  </si>
+  <si>
+    <t>Mirulal Murmu</t>
+  </si>
+  <si>
+    <t>Chholaki Devi</t>
+  </si>
+  <si>
+    <t>Shankar Kumar Ray</t>
+  </si>
+  <si>
+    <t>Prayag Ray</t>
+  </si>
+  <si>
+    <t>Suraj Kumar Ray</t>
+  </si>
+  <si>
+    <t>Mahangu Ray</t>
+  </si>
+  <si>
+    <t>Jwala Murmu</t>
+  </si>
+  <si>
+    <t>Badaki Devi</t>
+  </si>
+  <si>
+    <t>Jobamati Kumari</t>
+  </si>
+  <si>
+    <t>Budhu Murmu</t>
+  </si>
+  <si>
+    <t>Dasmi Kumari</t>
+  </si>
+  <si>
+    <t>Jiblal Murmu</t>
+  </si>
+  <si>
+    <t>Manoj Murmu</t>
+  </si>
+  <si>
+    <t>Hopan Murmu</t>
+  </si>
+  <si>
+    <t>Malti Devi</t>
+  </si>
+  <si>
+    <t>Karmati Kumari</t>
+  </si>
+  <si>
+    <t>Lopsa Murmu</t>
+  </si>
+  <si>
+    <t>Maloti Devi</t>
+  </si>
+  <si>
+    <t>Babita Kumari</t>
+  </si>
+  <si>
+    <t>Kedar Ray</t>
+  </si>
+  <si>
+    <t>Partima Devi</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t xml:space="preserve">85.20                    </t>
+  </si>
+  <si>
+    <t>Rupali Kumari</t>
+  </si>
+  <si>
+    <t>Nuna Tudu</t>
+  </si>
+  <si>
+    <t>Sanjhali Devi</t>
+  </si>
+  <si>
+    <t>Savita Kumari</t>
+  </si>
+  <si>
+    <t>Sitaram Tudu</t>
+  </si>
+  <si>
+    <t>337</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.40                    </t>
+  </si>
+  <si>
+    <t>Bindu Kumari</t>
+  </si>
+  <si>
+    <t>Lalbahadur Rana</t>
+  </si>
+  <si>
+    <t>316</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63.20                    </t>
+  </si>
+  <si>
+    <t>Ramdev Rana</t>
+  </si>
+  <si>
+    <t>349</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.80                    </t>
+  </si>
+  <si>
+    <t>Sanjit Kumar Rana</t>
+  </si>
+  <si>
+    <t>Puran Rana</t>
+  </si>
+  <si>
+    <t>Govind Soren</t>
+  </si>
+  <si>
+    <t>Nunuram Soren</t>
+  </si>
+  <si>
+    <t>Soniya Devi</t>
+  </si>
+  <si>
+    <t>Amar Turi</t>
+  </si>
+  <si>
+    <t>Tulshi Turi</t>
+  </si>
+  <si>
+    <t>280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.00                    </t>
+  </si>
+  <si>
+    <t>Namita Soren</t>
+  </si>
+  <si>
+    <t>Munulal Soren</t>
+  </si>
+  <si>
+    <t>Sukarmuni Devi</t>
+  </si>
+  <si>
+    <t>Manisha Kumari</t>
+  </si>
+  <si>
+    <t>Aditya Prasad Roy</t>
+  </si>
+  <si>
+    <t>432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">86.40                    </t>
+  </si>
+  <si>
+    <t>Ajay Baske</t>
+  </si>
+  <si>
+    <t>Prem Baske</t>
+  </si>
+  <si>
+    <t>Sukhi Devi</t>
+  </si>
+  <si>
+    <t>Gita Kumari</t>
+  </si>
+  <si>
+    <t>Kameshwar Rajak</t>
+  </si>
+  <si>
+    <t>Yashoda Kumari</t>
+  </si>
+  <si>
+    <t>Ganesh Rajak</t>
+  </si>
+  <si>
+    <t>Tenti Devi</t>
+  </si>
+  <si>
+    <t>311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62.20                    </t>
+  </si>
+  <si>
+    <t>Raja Turi</t>
+  </si>
+  <si>
+    <t>Arjun Turi</t>
+  </si>
+  <si>
+    <t>Ranju Devi</t>
+  </si>
+  <si>
+    <t>Uma Kumari</t>
+  </si>
+  <si>
+    <t>Mohan Rana</t>
+  </si>
+  <si>
+    <t>Baijnath Rana</t>
+  </si>
+  <si>
+    <t>278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.60                    </t>
+  </si>
+  <si>
+    <t>Sunil Hazam</t>
+  </si>
+  <si>
+    <t>328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.60                    </t>
+  </si>
+  <si>
+    <t>Mukesh Murmu</t>
+  </si>
+  <si>
+    <t>Madan Murmu</t>
+  </si>
+  <si>
+    <t>Sonodi Devi</t>
   </si>
 </sst>
 </file>
@@ -4202,7 +4473,44 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="3" tint="-0.499984740745262"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -4257,20 +4565,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C3636B2-7731-4DF4-A514-6384C85C902C}" name="Table1" displayName="Table1" ref="A1:H300" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4C3636B2-7731-4DF4-A514-6384C85C902C}" name="Table1" displayName="Table1" ref="A1:H300" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A1:H300" xr:uid="{4C3636B2-7731-4DF4-A514-6384C85C902C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H300">
     <sortCondition descending="1" ref="H1:H300"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3B965520-9A86-47F4-8492-5C18BF01C0F2}" name="Roll Number" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{3B965520-9A86-47F4-8492-5C18BF01C0F2}" name="Roll Number" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{D21E7D0F-03ED-42CC-8463-AD8F0711DE93}" name="Name"/>
     <tableColumn id="3" xr3:uid="{0717E7E9-B879-4D51-B732-B6BBC4547462}" name="Father's Name"/>
     <tableColumn id="4" xr3:uid="{2F8E9F2D-FFD7-4235-8937-9584BEFCC992}" name="Mother's Name"/>
     <tableColumn id="5" xr3:uid="{90A6FE32-6924-4675-832A-DCBF7798AC7D}" name="School / College Name"/>
-    <tableColumn id="6" xr3:uid="{4D40362B-9653-47FF-A763-BF863B30FEAF}" name="Marks" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9332C5FE-C099-491B-84AC-FE9751C0D6A0}" name="Result" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{2095A51D-CFCE-49A0-90D7-B21A399130D1}" name="Percentage" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{4D40362B-9653-47FF-A763-BF863B30FEAF}" name="Marks" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{9332C5FE-C099-491B-84AC-FE9751C0D6A0}" name="Result" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{2095A51D-CFCE-49A0-90D7-B21A399130D1}" name="Percentage" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{35E72ED5-3985-4AC7-B10F-4847163C523A}" name="Table2" displayName="Table2" ref="A1:H30" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:H30" xr:uid="{35E72ED5-3985-4AC7-B10F-4847163C523A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H30">
+    <sortCondition descending="1" ref="H1:H30"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{CD4AE622-9F6A-42BE-B06F-B58B506D3B52}" name="Roll Number" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{622F242A-3E88-413C-9C04-4A203741E164}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{5E6E1E6C-6849-4C3B-BC2B-5FC8ED0D33A0}" name="Father's Name"/>
+    <tableColumn id="4" xr3:uid="{462E374B-130D-48E1-86CD-033856E42D46}" name="Mother's Name"/>
+    <tableColumn id="5" xr3:uid="{034C3751-18AD-45A6-8367-786BA703F799}" name="School / College Name"/>
+    <tableColumn id="6" xr3:uid="{25C1C21A-8215-4702-8709-601DD218C6D2}" name="Marks" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{4764D613-6A6C-47D6-9B36-8D9B201A98F1}" name="Result" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{6BB2E97C-F197-4972-BA57-2A04DCC34CB7}" name="Percentage" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4541,8 +4869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12364,4 +12692,813 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F516E2D-91FB-4B08-876B-1149F20C79CB}">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D2" t="s">
+        <v>708</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1406</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D4" t="s">
+        <v>783</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D5" t="s">
+        <v>783</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>1383</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D7" t="s">
+        <v>659</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>963</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1419</v>
+      </c>
+      <c r="D8" t="s">
+        <v>708</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1411</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1397</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1400</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>772</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D13" t="s">
+        <v>877</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1448</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1415</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1441</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1442</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1433</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1443</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1445</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1446</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1447</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1387</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1388</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1171</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1408</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1409</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1410</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1427</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D22" t="s">
+        <v>797</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1453</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1019</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>1454</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1385</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1393</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1235</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>904</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1391</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1451</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1449</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1450</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1459</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1461</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1389</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D30" t="s">
+        <v>745</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1374</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>